<commit_message>
Add chromedriver and phantomjs
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="陈思平" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,21 +20,22 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="丁惠君" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="刁现芬" sheetId="13" state="visible" r:id="rId13"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="沈圆圆" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="陆敏华" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="张新宇" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="孙怡雯" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="李乔亮" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="齐素文" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="倪东" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="黄炳升" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="徐敏" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="雷柏英" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="常春起" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="陈雯雯" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="罗永祥" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="王倪传" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="张治国" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="董磊" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="周永进" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="陆敏华" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="张新宇" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="孙怡雯" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="李乔亮" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="齐素文" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="倪东" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="黄炳升" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="徐敏" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="雷柏英" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="常春起" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="陈雯雯" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="罗永祥" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="王倪传" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="张治国" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="董磊" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="597">
   <si>
     <t>题名</t>
   </si>
@@ -1043,6 +1044,15 @@
     <t>陈昕; 郭燕荣</t>
   </si>
   <si>
+    <t>融合超声影像动态评估中风偏瘫患者内侧腓肠肌状态</t>
+  </si>
+  <si>
+    <t>张旭东;钟昇;杨晓娟;周永进;杨万章;向云;王俊;王碧涵;杨钧鹏;陈昕</t>
+  </si>
+  <si>
+    <t>2017-03-30</t>
+  </si>
+  <si>
     <t>手背静脉图像ROI提取算法研究</t>
   </si>
   <si>
@@ -1085,6 +1095,15 @@
     <t>2016-03-22 10:47</t>
   </si>
   <si>
+    <t>基于对称区域生长算法的超声医学图像分割方法</t>
+  </si>
+  <si>
+    <t>张建;汪天富;李德玉;林江莉;唐红;饶莉</t>
+  </si>
+  <si>
+    <t>2007-06-25</t>
+  </si>
+  <si>
     <t>医学超声评价胎盘功能研究进展</t>
   </si>
   <si>
@@ -1139,9 +1158,36 @@
     <t>微计算机信息</t>
   </si>
   <si>
+    <t>新型医学信号处理实验平台的设计与实现</t>
+  </si>
+  <si>
+    <t>叶继伦; 顾家军; 刁现芬; 张旭; 汪天富</t>
+  </si>
+  <si>
+    <t>实验科学与技术</t>
+  </si>
+  <si>
+    <t>2017-02-28</t>
+  </si>
+  <si>
     <t>2011-06-15</t>
   </si>
   <si>
+    <t>超声医学图像滤波和对比度增强新方法</t>
+  </si>
+  <si>
+    <t>陈科; 林江莉; 李德玉; 汪天富</t>
+  </si>
+  <si>
+    <t>2007-04-25</t>
+  </si>
+  <si>
+    <t>基于形态学重构的超声医学图像滤波方法</t>
+  </si>
+  <si>
+    <t>张建炜; 林江莉; 李德玉; 汪天富</t>
+  </si>
+  <si>
     <t>基于先验概率和统计形状的前列腺超声图像自动分割方法</t>
   </si>
   <si>
@@ -1158,42 +1204,6 @@
   </si>
   <si>
     <t>2008-06-15</t>
-  </si>
-  <si>
-    <t>新型医学信号处理实验平台的设计与实现</t>
-  </si>
-  <si>
-    <t>叶继伦; 顾家军; 刁现芬; 张旭; 汪天富</t>
-  </si>
-  <si>
-    <t>实验科学与技术</t>
-  </si>
-  <si>
-    <t>2017-02-28</t>
-  </si>
-  <si>
-    <t>超声医学图像滤波和对比度增强新方法</t>
-  </si>
-  <si>
-    <t>陈科; 林江莉; 李德玉; 汪天富</t>
-  </si>
-  <si>
-    <t>2007-04-25</t>
-  </si>
-  <si>
-    <t>基于形态学重构的超声医学图像滤波方法</t>
-  </si>
-  <si>
-    <t>张建炜; 林江莉; 李德玉; 汪天富</t>
-  </si>
-  <si>
-    <t>2007-06-25</t>
-  </si>
-  <si>
-    <t>基于对称区域生长算法的超声医学图像分割方法</t>
-  </si>
-  <si>
-    <t>张建;汪天富;李德玉;林江莉;唐红;饶莉</t>
   </si>
   <si>
     <t>导语:中文认知加工的脑图谱研究</t>
@@ -1831,19 +1841,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <family val="3"/>
-      <sz val="9"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1871,28 +1874,8 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -2188,18 +2171,11 @@
   </sheetPr>
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5" outlineLevelCol="0"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="38.875"/>
-    <col customWidth="1" max="2" min="2" width="38.375"/>
-    <col customWidth="1" max="3" min="3" width="30.625"/>
-    <col customWidth="1" max="4" min="4" width="18.5"/>
-    <col customWidth="1" max="5" min="5" width="98.5"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -3665,7 +3641,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -3719,16 +3694,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B3" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C3" t="s">
         <v>284</v>
       </c>
       <c r="D3" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -3736,16 +3711,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B4" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C4" t="s">
         <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -3753,16 +3728,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B5" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C5" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D5" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -3770,16 +3745,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="B6" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C6" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="D6" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -3787,16 +3762,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="B7" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C7" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="D7" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -3804,16 +3779,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="B8" t="s">
+        <v>453</v>
+      </c>
+      <c r="C8" t="s">
         <v>450</v>
       </c>
-      <c r="C8" t="s">
-        <v>447</v>
-      </c>
       <c r="D8" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -3821,13 +3796,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B9" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D9" t="s">
         <v>293</v>
@@ -3838,16 +3813,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B10" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -3855,16 +3830,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B11" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C11" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="D11" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -3872,16 +3847,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="B12" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="C12" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="D12" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -3889,16 +3864,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
+        <v>469</v>
+      </c>
+      <c r="B13" t="s">
         <v>466</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>463</v>
       </c>
-      <c r="C13" t="s">
-        <v>460</v>
-      </c>
       <c r="D13" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -3906,16 +3881,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="B14" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C14" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="D14" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -3923,16 +3898,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B15" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="C15" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="D15" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -3957,16 +3932,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="B17" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -3974,16 +3949,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B18" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="C18" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="D18" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -3991,16 +3966,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B19" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="C19" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="D19" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -4008,13 +3983,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="B20" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C20" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D20" t="s">
         <v>85</v>
@@ -4095,16 +4070,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="B2" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="C2" t="s">
         <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -4182,13 +4157,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C2" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -4199,16 +4174,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="B3" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C3" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="D3" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -4252,16 +4227,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>362</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>363</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -4269,16 +4244,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C3" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D3" t="s">
-        <v>365</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -4286,16 +4261,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>488</v>
+        <v>368</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>369</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>370</v>
       </c>
       <c r="D4" t="s">
-        <v>490</v>
+        <v>375</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -4303,16 +4278,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -4320,16 +4295,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -4337,16 +4312,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>491</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>492</v>
       </c>
       <c r="C7" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>493</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -4354,16 +4329,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="C8" t="s">
-        <v>166</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -4371,16 +4346,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>238</v>
+        <v>175</v>
       </c>
       <c r="C9" t="s">
         <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>239</v>
+        <v>176</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -4388,16 +4363,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B10" t="s">
         <v>372</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>373</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>374</v>
-      </c>
-      <c r="D10" t="s">
-        <v>375</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -4405,16 +4380,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>166</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -4422,16 +4397,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C12" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -4439,16 +4414,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>238</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>239</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -4628,16 +4603,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="B10" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="C10" t="s">
         <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -4666,6 +4641,59 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4749,16 +4777,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="B5" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="C5" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="D5" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -4766,10 +4794,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="B6" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="C6" t="s">
         <v>245</v>
@@ -4783,16 +4811,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B7" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="C7" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="D7" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="E7" t="s">
         <v>247</v>
@@ -4803,7 +4831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4853,13 +4881,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C3" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D3" t="s">
         <v>145</v>
@@ -4870,16 +4898,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B4" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C4" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D4" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -4904,16 +4932,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B6" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C6" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D6" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -4972,10 +5000,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B10" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="C10" t="s">
         <v>245</v>
@@ -4992,7 +5020,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5025,16 +5053,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B2" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -5042,16 +5070,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="C3" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="D3" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -5059,16 +5087,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="C4" t="s">
         <v>94</v>
       </c>
       <c r="D4" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -5079,7 +5107,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5197,13 +5225,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B7" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C7" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D7" t="s">
         <v>293</v>
@@ -5251,7 +5279,536 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" t="s">
+        <v>292</v>
+      </c>
+      <c r="D4" t="s">
+        <v>293</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" t="s">
+        <v>295</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>296</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>297</v>
+      </c>
+      <c r="B10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>301</v>
+      </c>
+      <c r="B14" t="s">
+        <v>302</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>303</v>
+      </c>
+      <c r="B15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>305</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>306</v>
+      </c>
+      <c r="B17" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" t="s">
+        <v>308</v>
+      </c>
+      <c r="D17" t="s">
+        <v>309</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" t="s">
+        <v>308</v>
+      </c>
+      <c r="D18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B19" t="s">
+        <v>313</v>
+      </c>
+      <c r="C19" t="s">
+        <v>314</v>
+      </c>
+      <c r="D19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" t="s">
+        <v>217</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>218</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>316</v>
+      </c>
+      <c r="B22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C22" t="s">
+        <v>308</v>
+      </c>
+      <c r="D22" t="s">
+        <v>293</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" t="s">
+        <v>221</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>318</v>
+      </c>
+      <c r="B24" t="s">
+        <v>319</v>
+      </c>
+      <c r="C24" t="s">
+        <v>320</v>
+      </c>
+      <c r="D24" t="s">
+        <v>321</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>234</v>
+      </c>
+      <c r="B25" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>236</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>322</v>
+      </c>
+      <c r="B26" t="s">
+        <v>323</v>
+      </c>
+      <c r="C26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D26" t="s">
+        <v>325</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>326</v>
+      </c>
+      <c r="B27" t="s">
+        <v>327</v>
+      </c>
+      <c r="C27" t="s">
+        <v>328</v>
+      </c>
+      <c r="D27" t="s">
+        <v>329</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>330</v>
+      </c>
+      <c r="B28" t="s">
+        <v>327</v>
+      </c>
+      <c r="C28" t="s">
+        <v>328</v>
+      </c>
+      <c r="D28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>331</v>
+      </c>
+      <c r="B29" t="s">
+        <v>332</v>
+      </c>
+      <c r="C29" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>333</v>
+      </c>
+      <c r="B30" t="s">
+        <v>334</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>335</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5284,13 +5841,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B2" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C2" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D2" t="s">
         <v>293</v>
@@ -5301,16 +5858,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B3" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="C3" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="D3" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -5318,16 +5875,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B4" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="C4" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="D4" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -5335,16 +5892,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B5" t="s">
         <v>524</v>
       </c>
-      <c r="B5" t="s">
-        <v>521</v>
-      </c>
       <c r="C5" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D5" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -5352,16 +5909,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B6" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="C6" t="s">
         <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -5369,16 +5926,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="B7" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="C7" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="D7" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -5386,16 +5943,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="B8" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="C8" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="D8" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -5437,16 +5994,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="B11" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="C11" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="D11" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -5457,519 +6014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="13.5"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" t="s">
-        <v>285</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D3" t="s">
-        <v>289</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>290</v>
-      </c>
-      <c r="B4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C4" t="s">
-        <v>292</v>
-      </c>
-      <c r="D4" t="s">
-        <v>293</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" t="s">
-        <v>295</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>296</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>297</v>
-      </c>
-      <c r="B10" t="s">
-        <v>298</v>
-      </c>
-      <c r="C10" t="s">
-        <v>299</v>
-      </c>
-      <c r="D10" t="s">
-        <v>300</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" t="s">
-        <v>100</v>
-      </c>
-      <c r="C13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>301</v>
-      </c>
-      <c r="B14" t="s">
-        <v>302</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>207</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B15" t="s">
-        <v>304</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>305</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>306</v>
-      </c>
-      <c r="B17" t="s">
-        <v>307</v>
-      </c>
-      <c r="C17" t="s">
-        <v>308</v>
-      </c>
-      <c r="D17" t="s">
-        <v>309</v>
-      </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>310</v>
-      </c>
-      <c r="B18" t="s">
-        <v>311</v>
-      </c>
-      <c r="C18" t="s">
-        <v>308</v>
-      </c>
-      <c r="D18" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>312</v>
-      </c>
-      <c r="B19" t="s">
-        <v>313</v>
-      </c>
-      <c r="C19" t="s">
-        <v>314</v>
-      </c>
-      <c r="D19" t="s">
-        <v>315</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>216</v>
-      </c>
-      <c r="B20" t="s">
-        <v>217</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" t="s">
-        <v>218</v>
-      </c>
-      <c r="E20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>208</v>
-      </c>
-      <c r="B21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s">
-        <v>210</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>316</v>
-      </c>
-      <c r="B22" t="s">
-        <v>317</v>
-      </c>
-      <c r="C22" t="s">
-        <v>308</v>
-      </c>
-      <c r="D22" t="s">
-        <v>293</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>219</v>
-      </c>
-      <c r="B23" t="s">
-        <v>220</v>
-      </c>
-      <c r="C23" t="s">
-        <v>192</v>
-      </c>
-      <c r="D23" t="s">
-        <v>221</v>
-      </c>
-      <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>318</v>
-      </c>
-      <c r="B24" t="s">
-        <v>319</v>
-      </c>
-      <c r="C24" t="s">
-        <v>320</v>
-      </c>
-      <c r="D24" t="s">
-        <v>321</v>
-      </c>
-      <c r="E24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>234</v>
-      </c>
-      <c r="B25" t="s">
-        <v>235</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>236</v>
-      </c>
-      <c r="E25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>322</v>
-      </c>
-      <c r="B26" t="s">
-        <v>323</v>
-      </c>
-      <c r="C26" t="s">
-        <v>324</v>
-      </c>
-      <c r="D26" t="s">
-        <v>325</v>
-      </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>326</v>
-      </c>
-      <c r="B27" t="s">
-        <v>327</v>
-      </c>
-      <c r="C27" t="s">
-        <v>328</v>
-      </c>
-      <c r="D27" t="s">
-        <v>329</v>
-      </c>
-      <c r="E27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>330</v>
-      </c>
-      <c r="B28" t="s">
-        <v>327</v>
-      </c>
-      <c r="C28" t="s">
-        <v>328</v>
-      </c>
-      <c r="D28" t="s">
-        <v>143</v>
-      </c>
-      <c r="E28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>331</v>
-      </c>
-      <c r="B29" t="s">
-        <v>332</v>
-      </c>
-      <c r="C29" t="s">
-        <v>245</v>
-      </c>
-      <c r="D29" t="s">
-        <v>246</v>
-      </c>
-      <c r="E29" t="s">
-        <v>247</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6019,16 +6064,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="B3" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -6087,16 +6132,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="B7" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -6138,16 +6183,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>366</v>
+        <v>381</v>
       </c>
       <c r="B10" t="s">
-        <v>367</v>
+        <v>382</v>
       </c>
       <c r="C10" t="s">
         <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>368</v>
+        <v>383</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -6155,16 +6200,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B11" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="C11" t="s">
         <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -6189,10 +6234,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="B13" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="C13" t="s">
         <v>142</v>
@@ -6209,7 +6254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6242,16 +6287,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -6259,13 +6304,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="B3" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="C3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D3" t="s">
         <v>309</v>
@@ -6276,16 +6321,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C4" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D4" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -6296,7 +6341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6329,16 +6374,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="B2" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="C2" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="D2" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -6346,16 +6391,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="B3" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="C3" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="D3" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -6363,16 +6408,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="B4" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="C4" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="D4" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -6380,89 +6425,19 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B5" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="C5" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="D5" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="E5" t="s">
         <v>247</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6503,16 +6478,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>563</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>564</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>565</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>566</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -6520,16 +6495,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>567</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>568</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>569</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>570</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -6546,7 +6521,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6573,18 +6548,35 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B2" t="s">
+        <v>567</v>
+      </c>
+      <c r="C2" t="s">
+        <v>568</v>
+      </c>
+      <c r="D2" t="s">
+        <v>569</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>570</v>
+      </c>
+      <c r="B3" t="s">
         <v>571</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>572</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>573</v>
       </c>
-      <c r="D2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6635,7 +6627,7 @@
         <v>576</v>
       </c>
       <c r="D2" t="s">
-        <v>577</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -6679,13 +6671,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" t="s">
         <v>578</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>579</v>
-      </c>
-      <c r="C2" t="s">
-        <v>569</v>
       </c>
       <c r="D2" t="s">
         <v>580</v>
@@ -6732,16 +6724,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>581</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>582</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>572</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
+        <v>583</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -6758,7 +6750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6785,86 +6777,18 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>581</v>
+        <v>294</v>
       </c>
       <c r="B2" t="s">
-        <v>582</v>
+        <v>295</v>
       </c>
       <c r="C2" t="s">
-        <v>583</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>584</v>
+        <v>296</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>395</v>
-      </c>
-      <c r="B3" t="s">
-        <v>396</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>397</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>585</v>
-      </c>
-      <c r="B4" t="s">
-        <v>586</v>
-      </c>
-      <c r="C4" t="s">
-        <v>583</v>
-      </c>
-      <c r="D4" t="s">
-        <v>587</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>588</v>
-      </c>
-      <c r="B5" t="s">
-        <v>589</v>
-      </c>
-      <c r="C5" t="s">
-        <v>583</v>
-      </c>
-      <c r="D5" t="s">
-        <v>590</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>591</v>
-      </c>
-      <c r="B6" t="s">
-        <v>592</v>
-      </c>
-      <c r="C6" t="s">
-        <v>583</v>
-      </c>
-      <c r="D6" t="s">
-        <v>593</v>
-      </c>
-      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -6923,16 +6847,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C3" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D3" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -6940,16 +6864,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="C4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="D4" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -6991,16 +6915,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C7" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -7025,16 +6949,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B9" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C9" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D9" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -7076,16 +7000,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>350</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>351</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>352</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -7093,16 +7017,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -7110,16 +7034,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
         <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -7127,16 +7051,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -7144,16 +7068,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>347</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>348</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>349</v>
+        <v>116</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -7161,16 +7085,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>353</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>354</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>355</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -7178,16 +7102,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>350</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>351</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>324</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>352</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -7195,16 +7119,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>356</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>357</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>324</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>358</v>
       </c>
       <c r="E19" t="s">
         <v>9</v>
@@ -7212,16 +7136,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>353</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>354</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>355</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
         <v>9</v>
@@ -7229,16 +7153,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>359</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>360</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>361</v>
       </c>
       <c r="E21" t="s">
         <v>9</v>
@@ -7246,16 +7170,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>356</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>357</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>324</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>358</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
         <v>9</v>
@@ -7280,16 +7204,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B24" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>324</v>
       </c>
       <c r="D24" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="E24" t="s">
         <v>9</v>
@@ -7297,16 +7221,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>365</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>366</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>367</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
@@ -7314,16 +7238,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
@@ -7331,16 +7255,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
         <v>9</v>
@@ -7348,16 +7272,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
         <v>9</v>
@@ -7365,13 +7289,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>362</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
-        <v>363</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>364</v>
+        <v>130</v>
       </c>
       <c r="D29" t="s">
         <v>145</v>
@@ -7382,16 +7306,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="B30" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C30" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="D30" t="s">
-        <v>365</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
@@ -7399,16 +7323,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>371</v>
       </c>
       <c r="B31" t="s">
-        <v>175</v>
+        <v>372</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>373</v>
       </c>
       <c r="D31" t="s">
-        <v>176</v>
+        <v>374</v>
       </c>
       <c r="E31" t="s">
         <v>9</v>
@@ -7416,16 +7340,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>368</v>
       </c>
       <c r="B32" t="s">
-        <v>178</v>
+        <v>369</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>370</v>
       </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>375</v>
       </c>
       <c r="E32" t="s">
         <v>9</v>
@@ -7433,16 +7357,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B33" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E33" t="s">
         <v>9</v>
@@ -7450,16 +7374,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="E34" t="s">
         <v>9</v>
@@ -7467,16 +7391,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C35" t="s">
-        <v>203</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E35" t="s">
         <v>9</v>
@@ -7484,16 +7408,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>192</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
         <v>9</v>
@@ -7501,16 +7425,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>203</v>
       </c>
       <c r="D37" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E37" t="s">
         <v>9</v>
@@ -7518,16 +7442,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="B38" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>192</v>
       </c>
       <c r="D38" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="E38" t="s">
         <v>9</v>
@@ -7535,16 +7459,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B39" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>207</v>
       </c>
       <c r="E39" t="s">
         <v>9</v>
@@ -7552,16 +7476,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="B40" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
       </c>
       <c r="D40" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="E40" t="s">
         <v>9</v>
@@ -7569,16 +7493,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C41" t="s">
-        <v>192</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
-        <v>221</v>
+        <v>85</v>
       </c>
       <c r="E41" t="s">
         <v>9</v>
@@ -7586,16 +7510,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>366</v>
+        <v>216</v>
       </c>
       <c r="B42" t="s">
-        <v>367</v>
+        <v>217</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="D42" t="s">
-        <v>368</v>
+        <v>218</v>
       </c>
       <c r="E42" t="s">
         <v>9</v>
@@ -7603,16 +7527,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="B43" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="C43" t="s">
         <v>35</v>
       </c>
       <c r="D43" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="E43" t="s">
         <v>9</v>
@@ -7620,16 +7544,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>228</v>
+        <v>379</v>
       </c>
       <c r="B44" t="s">
-        <v>229</v>
+        <v>380</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>230</v>
+        <v>352</v>
       </c>
       <c r="E44" t="s">
         <v>9</v>
@@ -7637,16 +7561,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B45" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C45" t="s">
-        <v>42</v>
+        <v>192</v>
       </c>
       <c r="D45" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="E45" t="s">
         <v>9</v>
@@ -7654,16 +7578,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>234</v>
+        <v>381</v>
       </c>
       <c r="B46" t="s">
-        <v>235</v>
+        <v>382</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
-        <v>236</v>
+        <v>383</v>
       </c>
       <c r="E46" t="s">
         <v>9</v>
@@ -7671,16 +7595,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>384</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>385</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>35</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>386</v>
       </c>
       <c r="E47" t="s">
         <v>9</v>
@@ -7688,16 +7612,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>153</v>
+        <v>228</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>229</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
-        <v>155</v>
+        <v>230</v>
       </c>
       <c r="E48" t="s">
         <v>9</v>
@@ -7705,16 +7629,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
       <c r="B49" t="s">
-        <v>165</v>
+        <v>232</v>
       </c>
       <c r="C49" t="s">
-        <v>166</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>167</v>
+        <v>233</v>
       </c>
       <c r="E49" t="s">
         <v>9</v>
@@ -7722,16 +7646,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>234</v>
       </c>
       <c r="B50" t="s">
-        <v>169</v>
+        <v>235</v>
       </c>
       <c r="C50" t="s">
-        <v>166</v>
+        <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>170</v>
+        <v>236</v>
       </c>
       <c r="E50" t="s">
         <v>9</v>
@@ -7739,16 +7663,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>237</v>
+        <v>146</v>
       </c>
       <c r="B51" t="s">
-        <v>238</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>239</v>
+        <v>147</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
@@ -7756,188 +7680,309 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>262</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>263</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>258</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>259</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>247</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>248</v>
+        <v>164</v>
       </c>
       <c r="B53" t="s">
-        <v>249</v>
+        <v>165</v>
       </c>
       <c r="C53" t="s">
-        <v>250</v>
+        <v>166</v>
       </c>
       <c r="D53" t="s">
-        <v>251</v>
+        <v>167</v>
       </c>
       <c r="E53" t="s">
-        <v>247</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>252</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
-        <v>253</v>
+        <v>169</v>
       </c>
       <c r="C54" t="s">
-        <v>250</v>
+        <v>166</v>
       </c>
       <c r="D54" t="s">
-        <v>251</v>
+        <v>170</v>
       </c>
       <c r="E54" t="s">
-        <v>247</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="B55" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="C55" t="s">
-        <v>258</v>
+        <v>101</v>
       </c>
       <c r="D55" t="s">
-        <v>259</v>
+        <v>239</v>
       </c>
       <c r="E55" t="s">
-        <v>247</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B56" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C56" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="D56" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="E56" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B57" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="C57" t="s">
-        <v>276</v>
+        <v>250</v>
       </c>
       <c r="D57" t="s">
-        <v>277</v>
+        <v>251</v>
       </c>
       <c r="E57" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>278</v>
+        <v>252</v>
       </c>
       <c r="B58" t="s">
-        <v>279</v>
+        <v>253</v>
       </c>
       <c r="C58" t="s">
-        <v>280</v>
+        <v>250</v>
       </c>
       <c r="D58" t="s">
-        <v>281</v>
+        <v>251</v>
       </c>
       <c r="E58" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>372</v>
+        <v>256</v>
       </c>
       <c r="B59" t="s">
-        <v>373</v>
+        <v>257</v>
       </c>
       <c r="C59" t="s">
-        <v>374</v>
+        <v>258</v>
       </c>
       <c r="D59" t="s">
-        <v>375</v>
+        <v>259</v>
       </c>
       <c r="E59" t="s">
-        <v>9</v>
+        <v>247</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>376</v>
+        <v>269</v>
       </c>
       <c r="B60" t="s">
-        <v>377</v>
+        <v>270</v>
       </c>
       <c r="C60" t="s">
-        <v>35</v>
+        <v>271</v>
       </c>
       <c r="D60" t="s">
-        <v>378</v>
+        <v>272</v>
       </c>
       <c r="E60" t="s">
-        <v>9</v>
+        <v>273</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>379</v>
+        <v>269</v>
       </c>
       <c r="B61" t="s">
-        <v>380</v>
+        <v>270</v>
       </c>
       <c r="C61" t="s">
-        <v>35</v>
+        <v>276</v>
       </c>
       <c r="D61" t="s">
-        <v>381</v>
+        <v>277</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>382</v>
+        <v>278</v>
       </c>
       <c r="B62" t="s">
-        <v>383</v>
+        <v>279</v>
       </c>
       <c r="C62" t="s">
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="D62" t="s">
-        <v>381</v>
+        <v>281</v>
       </c>
       <c r="E62" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C2" t="s">
+        <v>586</v>
+      </c>
+      <c r="D2" t="s">
+        <v>587</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>400</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>588</v>
+      </c>
+      <c r="B4" t="s">
+        <v>589</v>
+      </c>
+      <c r="C4" t="s">
+        <v>586</v>
+      </c>
+      <c r="D4" t="s">
+        <v>590</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>591</v>
+      </c>
+      <c r="B5" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" t="s">
+        <v>586</v>
+      </c>
+      <c r="D5" t="s">
+        <v>593</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>594</v>
+      </c>
+      <c r="B6" t="s">
+        <v>595</v>
+      </c>
+      <c r="C6" t="s">
+        <v>586</v>
+      </c>
+      <c r="D6" t="s">
+        <v>596</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -7979,16 +8024,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C2" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="D2" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -8102,13 +8147,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C2" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="D2" t="s">
         <v>131</v>
@@ -8136,16 +8181,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B4" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C4" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="D4" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -8153,16 +8198,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B5" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -8187,16 +8232,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="B7" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="C7" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="D7" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -8204,16 +8249,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B8" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C8" t="s">
         <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -8221,16 +8266,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B9" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C9" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="D9" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -8274,16 +8319,16 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B2" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -8308,10 +8353,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B4" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -8325,16 +8370,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B5" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -8359,16 +8404,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B7" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -8376,16 +8421,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>416</v>
+        <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>417</v>
+        <v>372</v>
       </c>
       <c r="C8" t="s">
-        <v>130</v>
+        <v>373</v>
       </c>
       <c r="D8" t="s">
-        <v>418</v>
+        <v>374</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -8402,7 +8447,7 @@
         <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>300</v>
+        <v>421</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -8410,16 +8455,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>422</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>423</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>300</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -8427,16 +8472,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>421</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>422</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>423</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -8461,16 +8506,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>427</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>428</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>429</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -8478,16 +8523,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>427</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>428</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>429</v>
+        <v>135</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -8501,7 +8546,7 @@
         <v>431</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>432</v>
@@ -8518,10 +8563,10 @@
         <v>434</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>435</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -8529,16 +8574,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>372</v>
+        <v>436</v>
       </c>
       <c r="B17" t="s">
-        <v>373</v>
+        <v>437</v>
       </c>
       <c r="C17" t="s">
-        <v>374</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>375</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -8805,10 +8850,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B4" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C4" t="s">
         <v>130</v>
@@ -8822,16 +8867,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -8856,10 +8901,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B7" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -8873,16 +8918,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -8890,16 +8935,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B9" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C9" t="s">
         <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -8907,10 +8952,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="B10" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C10" t="s">
         <v>26</v>
@@ -8924,16 +8969,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="B11" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -8941,16 +8986,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="B12" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C12" t="s">
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
@@ -8958,16 +9003,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C13" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D13" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -8975,16 +9020,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
+        <v>371</v>
+      </c>
+      <c r="B14" t="s">
         <v>372</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>373</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>374</v>
-      </c>
-      <c r="D14" t="s">
-        <v>375</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>

</xml_diff>